<commit_message>
added validation to rule specifications worksheet
</commit_message>
<xml_diff>
--- a/src/main/resources/rule specifications.xlsx
+++ b/src/main/resources/rule specifications.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\dva-sop-api\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\dva-sop-api\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="23880"/>
   </bookViews>
   <sheets>
     <sheet name="RH" sheetId="1" r:id="rId1"/>
     <sheet name="BoP" sheetId="3" r:id="rId2"/>
+    <sheet name="Lookups" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="32">
   <si>
     <t>Condition</t>
   </si>
@@ -118,6 +120,9 @@
   </si>
   <si>
     <t>6(m)(i), 6(gg)(i)</t>
+  </si>
+  <si>
+    <t>Royal Australian Air Force</t>
   </si>
 </sst>
 </file>
@@ -175,7 +180,83 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -186,6 +267,42 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J18" totalsRowShown="0">
+  <autoFilter ref="A1:J18"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Condition"/>
+    <tableColumn id="2" name="Instrument ID"/>
+    <tableColumn id="3" name="Factor References"/>
+    <tableColumn id="4" name="Service Branch"/>
+    <tableColumn id="5" name="Rank"/>
+    <tableColumn id="6" name="CFTS weeks"/>
+    <tableColumn id="7" name="Accumulation Rate per week"/>
+    <tableColumn id="8" name="Accumulation Unit"/>
+    <tableColumn id="9" name="RH operational services days "/>
+    <tableColumn id="10" name="RH operational service test period (years)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H13" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:H13"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Condition"/>
+    <tableColumn id="2" name="Instrument ID" dataDxfId="4"/>
+    <tableColumn id="3" name="Factor References" dataDxfId="3"/>
+    <tableColumn id="4" name="Service Branch" dataDxfId="2"/>
+    <tableColumn id="5" name="Rank" dataDxfId="1"/>
+    <tableColumn id="6" name="CFTS weeks"/>
+    <tableColumn id="7" name="Accumulation Rate per week"/>
+    <tableColumn id="8" name="Accumulation Unit"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -487,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,8 +1161,38 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection insertRows="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0"/>
+  <dataValidations count="2">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:J1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:G1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lookups!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lookups!$B$1:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1054,22 +1201,22 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.140625" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="35.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1408,6 +1555,77 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:G1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lookups!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lookups!$B$1:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>